<commit_message>
update root keys for output json
</commit_message>
<xml_diff>
--- a/test/data/file.xlsx
+++ b/test/data/file.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>sourcecontrol</t>
+  </si>
   <si>
     <t>a,1</t>
   </si>
@@ -20,10 +23,10 @@
     <t>b,1</t>
   </si>
   <si>
+    <t>nombre2</t>
+  </si>
+  <si>
     <t>s,3</t>
-  </si>
-  <si>
-    <t>nombre2</t>
   </si>
   <si>
     <t>d,2</t>
@@ -33,7 +36,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -43,6 +46,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -58,11 +62,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -308,12 +315,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -321,8 +328,13 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="M6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>